<commit_message>
Add turtle graphical practice
</commit_message>
<xml_diff>
--- a/Automated-Emails/people.xlsx
+++ b/Automated-Emails/people.xlsx
@@ -38,7 +38,7 @@
         <color indexed="15"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>ypddjuio@yomail.info</t>
+      <t>anhhuy9900@yopmail.com</t>
     </r>
   </si>
   <si>
@@ -55,7 +55,7 @@
         <color indexed="15"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>kawnlyiw@supere.ml</t>
+      <t>anhhuy9901@yopmail.com</t>
     </r>
   </si>
   <si>
@@ -75,7 +75,7 @@
         <color indexed="15"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t>pythonprocourse2@gmail.com</t>
+      <t>nhahuy29051990@gmail.com</t>
     </r>
   </si>
 </sst>
@@ -1624,9 +1624,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="ypddjuio@yomail.info"/>
-    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="kawnlyiw@supere.ml"/>
-    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display="pythonprocourse2@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display="anhhuy9900@yopmail.com"/>
+    <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display="anhhuy9901@yopmail.com"/>
+    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display="nhahuy29051990@gmail.com"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>